<commit_message>
working on beta 4.0
</commit_message>
<xml_diff>
--- a/application/views/rpt/ru/doc/schet.xlsx
+++ b/application/views/rpt/ru/doc/schet.xlsx
@@ -239,7 +239,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -552,37 +552,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -599,143 +573,137 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1009,7 +977,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1020,7 +988,7 @@
   <dimension ref="B1:R31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q21:R22"/>
+      <selection activeCell="U15" sqref="U15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1046,541 +1014,541 @@
   <sheetData>
     <row r="1" spans="2:18" ht="409.6" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:18" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
     </row>
     <row r="3" spans="2:18" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
-      <c r="O3" s="38"/>
-      <c r="P3" s="38"/>
-      <c r="Q3" s="38"/>
-      <c r="R3" s="38"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
     </row>
     <row r="4" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="39"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="24"/>
     </row>
     <row r="5" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="40" t="s">
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="41"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="44" t="s">
+      <c r="K5" s="26"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="N5" s="44"/>
-      <c r="O5" s="44"/>
-      <c r="P5" s="44"/>
-      <c r="Q5" s="44"/>
-      <c r="R5" s="44"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
     </row>
     <row r="6" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="51"/>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="31" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="K6" s="32"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="43" t="s">
+      <c r="K6" s="29"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="N6" s="43"/>
-      <c r="O6" s="43"/>
-      <c r="P6" s="43"/>
-      <c r="Q6" s="43"/>
-      <c r="R6" s="43"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="21"/>
+      <c r="R6" s="21"/>
     </row>
     <row r="7" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="36"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="19"/>
       <c r="J7" s="6"/>
-      <c r="K7" s="29"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="43"/>
-      <c r="N7" s="43"/>
-      <c r="O7" s="43"/>
-      <c r="P7" s="43"/>
-      <c r="Q7" s="43"/>
-      <c r="R7" s="43"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="21"/>
     </row>
     <row r="8" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30" t="s">
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="31" t="s">
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="K8" s="32"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="43" t="s">
+      <c r="K8" s="29"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="N8" s="43"/>
-      <c r="O8" s="43"/>
-      <c r="P8" s="43"/>
-      <c r="Q8" s="43"/>
-      <c r="R8" s="43"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="21"/>
     </row>
     <row r="9" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="47"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="10"/>
       <c r="J9" s="7"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="43"/>
-      <c r="N9" s="43"/>
-      <c r="O9" s="43"/>
-      <c r="P9" s="43"/>
-      <c r="Q9" s="43"/>
-      <c r="R9" s="43"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="21"/>
     </row>
     <row r="10" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="36"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="19"/>
       <c r="J10" s="6"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="43"/>
-      <c r="N10" s="43"/>
-      <c r="O10" s="43"/>
-      <c r="P10" s="43"/>
-      <c r="Q10" s="43"/>
-      <c r="R10" s="43"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="21"/>
     </row>
     <row r="11" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="2:18" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="28"/>
-      <c r="Q12" s="28"/>
-      <c r="R12" s="28"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="32"/>
+      <c r="N12" s="32"/>
+      <c r="O12" s="32"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="32"/>
+      <c r="R12" s="32"/>
     </row>
     <row r="13" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="24" t="s">
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="24"/>
-      <c r="L14" s="24"/>
-      <c r="M14" s="24"/>
-      <c r="N14" s="24"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="24"/>
-      <c r="R14" s="24"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="37"/>
+      <c r="M14" s="37"/>
+      <c r="N14" s="37"/>
+      <c r="O14" s="37"/>
+      <c r="P14" s="37"/>
+      <c r="Q14" s="37"/>
+      <c r="R14" s="37"/>
     </row>
     <row r="15" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="24" t="s">
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="24"/>
-      <c r="M15" s="24"/>
-      <c r="N15" s="24"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="24"/>
-      <c r="R15" s="24"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="37"/>
+      <c r="N15" s="37"/>
+      <c r="O15" s="37"/>
+      <c r="P15" s="37"/>
+      <c r="Q15" s="37"/>
+      <c r="R15" s="37"/>
     </row>
     <row r="16" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
     </row>
     <row r="17" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="25"/>
-      <c r="O17" s="25"/>
-      <c r="P17" s="25"/>
-      <c r="Q17" s="25"/>
-      <c r="R17" s="25"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="38"/>
+      <c r="N17" s="38"/>
+      <c r="O17" s="38"/>
+      <c r="P17" s="38"/>
+      <c r="Q17" s="38"/>
+      <c r="R17" s="38"/>
     </row>
     <row r="18" spans="2:18" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="27" t="s">
+      <c r="C18" s="39"/>
+      <c r="D18" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
       <c r="H18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I18" s="27" t="s">
+      <c r="I18" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="J18" s="27"/>
-      <c r="K18" s="27" t="s">
+      <c r="J18" s="40"/>
+      <c r="K18" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="L18" s="27"/>
-      <c r="M18" s="27"/>
-      <c r="N18" s="27" t="s">
+      <c r="L18" s="40"/>
+      <c r="M18" s="40"/>
+      <c r="N18" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="O18" s="27"/>
-      <c r="P18" s="27"/>
-      <c r="Q18" s="23" t="s">
+      <c r="O18" s="40"/>
+      <c r="P18" s="40"/>
+      <c r="Q18" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="R18" s="23"/>
+      <c r="R18" s="35"/>
     </row>
     <row r="19" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="18" t="s">
+      <c r="C19" s="42"/>
+      <c r="D19" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
       <c r="H19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I19" s="18" t="s">
+      <c r="I19" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18" t="s">
+      <c r="J19" s="43"/>
+      <c r="K19" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18" t="s">
+      <c r="L19" s="43"/>
+      <c r="M19" s="43"/>
+      <c r="N19" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="19" t="s">
+      <c r="O19" s="43"/>
+      <c r="P19" s="43"/>
+      <c r="Q19" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="R19" s="19"/>
+      <c r="R19" s="44"/>
     </row>
     <row r="20" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="21" t="s">
+      <c r="C20" s="45"/>
+      <c r="D20" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46"/>
       <c r="H20" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I20" s="20" t="s">
+      <c r="I20" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="J20" s="20"/>
-      <c r="K20" s="22" t="s">
+      <c r="J20" s="45"/>
+      <c r="K20" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="L20" s="22"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="16" t="s">
+      <c r="L20" s="47"/>
+      <c r="M20" s="47"/>
+      <c r="N20" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="O20" s="16"/>
-      <c r="P20" s="16"/>
-      <c r="Q20" s="16" t="s">
+      <c r="O20" s="41"/>
+      <c r="P20" s="41"/>
+      <c r="Q20" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="R20" s="16"/>
+      <c r="R20" s="41"/>
     </row>
     <row r="21" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H21" s="12" t="s">
+      <c r="H21" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12"/>
-      <c r="O21" s="12"/>
-      <c r="Q21" s="54" t="s">
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="36"/>
+      <c r="O21" s="36"/>
+      <c r="Q21" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="R21" s="55"/>
+      <c r="R21" s="49"/>
     </row>
     <row r="22" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H22" s="8" t="s">
+      <c r="H22" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
-      <c r="Q22" s="54" t="s">
+      <c r="I22" s="36"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="36"/>
+      <c r="M22" s="36"/>
+      <c r="N22" s="36"/>
+      <c r="O22" s="36"/>
+      <c r="Q22" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="R22" s="55"/>
+      <c r="R22" s="49"/>
     </row>
     <row r="23" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H23" s="13" t="s">
+      <c r="H23" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="14" t="s">
+      <c r="I23" s="50"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="50"/>
+      <c r="L23" s="50"/>
+      <c r="M23" s="50"/>
+      <c r="N23" s="50"/>
+      <c r="O23" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="P23" s="14"/>
-      <c r="Q23" s="14"/>
-      <c r="R23" s="14"/>
+      <c r="P23" s="51"/>
+      <c r="Q23" s="51"/>
+      <c r="R23" s="51"/>
     </row>
     <row r="24" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="15"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="52"/>
+      <c r="M24" s="52"/>
+      <c r="N24" s="52"/>
+      <c r="O24" s="52"/>
+      <c r="P24" s="52"/>
+      <c r="Q24" s="52"/>
+      <c r="R24" s="52"/>
     </row>
     <row r="25" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="9"/>
-      <c r="P25" s="9"/>
-      <c r="Q25" s="9"/>
-      <c r="R25" s="9"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="53"/>
+      <c r="I25" s="53"/>
+      <c r="J25" s="53"/>
+      <c r="K25" s="53"/>
+      <c r="L25" s="53"/>
+      <c r="M25" s="53"/>
+      <c r="N25" s="53"/>
+      <c r="O25" s="53"/>
+      <c r="P25" s="53"/>
+      <c r="Q25" s="53"/>
+      <c r="R25" s="53"/>
     </row>
     <row r="26" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="9" t="s">
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="34"/>
+      <c r="J27" s="34"/>
+      <c r="K27" s="34"/>
+      <c r="L27" s="34"/>
+      <c r="M27" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="N27" s="9"/>
-      <c r="O27" s="9"/>
-      <c r="P27" s="9"/>
-      <c r="Q27" s="9"/>
-      <c r="R27" s="9"/>
+      <c r="N27" s="53"/>
+      <c r="O27" s="53"/>
+      <c r="P27" s="53"/>
+      <c r="Q27" s="53"/>
+      <c r="R27" s="53"/>
     </row>
     <row r="28" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
-      <c r="L28" s="11"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="48"/>
+      <c r="I28" s="48"/>
+      <c r="J28" s="48"/>
+      <c r="K28" s="48"/>
+      <c r="L28" s="48"/>
     </row>
     <row r="29" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="9" t="s">
+      <c r="C29" s="36"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="34"/>
+      <c r="J29" s="34"/>
+      <c r="K29" s="34"/>
+      <c r="L29" s="34"/>
+      <c r="M29" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="9"/>
-      <c r="R29" s="9"/>
+      <c r="N29" s="53"/>
+      <c r="O29" s="53"/>
+      <c r="P29" s="53"/>
+      <c r="Q29" s="53"/>
+      <c r="R29" s="53"/>
     </row>
     <row r="30" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="48"/>
       <c r="I30" s="4"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
-      <c r="L30" s="11"/>
+      <c r="J30" s="48"/>
+      <c r="K30" s="48"/>
+      <c r="L30" s="48"/>
     </row>
     <row r="31" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I31" s="5" t="s">
@@ -1589,24 +1557,35 @@
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="B2:R2"/>
-    <mergeCell ref="B3:R3"/>
-    <mergeCell ref="C4:Q4"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="M6:R7"/>
-    <mergeCell ref="M5:R5"/>
-    <mergeCell ref="B5:I6"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B12:R12"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="K9:L10"/>
-    <mergeCell ref="B10:I10"/>
-    <mergeCell ref="B9:I9"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="M8:R10"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="M29:R29"/>
+    <mergeCell ref="G29:L29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="J30:L30"/>
+    <mergeCell ref="G28:L28"/>
+    <mergeCell ref="H21:O21"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="H22:O22"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="H23:N23"/>
+    <mergeCell ref="O23:R23"/>
+    <mergeCell ref="B24:R24"/>
+    <mergeCell ref="B25:R25"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="M27:R27"/>
+    <mergeCell ref="G27:L27"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="N20:P20"/>
     <mergeCell ref="Q18:R18"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="E14:R14"/>
@@ -1619,38 +1598,27 @@
     <mergeCell ref="I18:J18"/>
     <mergeCell ref="K18:M18"/>
     <mergeCell ref="N18:P18"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="N19:P19"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:G20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="G28:L28"/>
-    <mergeCell ref="H21:O21"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="H22:O22"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="H23:N23"/>
-    <mergeCell ref="O23:R23"/>
-    <mergeCell ref="B24:R24"/>
-    <mergeCell ref="B25:R25"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="M27:R27"/>
-    <mergeCell ref="G27:L27"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="M29:R29"/>
-    <mergeCell ref="G29:L29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="J30:L30"/>
+    <mergeCell ref="B12:R12"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="K9:L10"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B2:R2"/>
+    <mergeCell ref="B3:R3"/>
+    <mergeCell ref="C4:Q4"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="M6:R7"/>
+    <mergeCell ref="M5:R5"/>
+    <mergeCell ref="B9:I9"/>
+    <mergeCell ref="B5:I6"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="M8:R10"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="90" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="90" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
bugfix payment bill wrong company_code
</commit_message>
<xml_diff>
--- a/application/views/rpt/ru/doc/schet.xlsx
+++ b/application/views/rpt/ru/doc/schet.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\iSell\www\isell\application\views\rpt\ru\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="30" windowWidth="7455" windowHeight="6240"/>
   </bookViews>
@@ -127,9 +132,6 @@
     <t xml:space="preserve">{$v-&gt;p-&gt;company_name}  </t>
   </si>
   <si>
-    <t>{$v-&gt;a-&gt;company_vat_id}  / {$v-&gt;a-&gt;company_vat_licence_id}</t>
-  </si>
-  <si>
     <t>{$v-&gt;rows[]-&gt;product_code}</t>
   </si>
   <si>
@@ -176,12 +178,15 @@
   </si>
   <si>
     <t>{$v-&gt;rows[]-&gt;product_sum}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;p-&gt;company_vat_id}  / {$v-&gt;p-&gt;company_vat_licence_id}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0;\-0;\-"/>
     <numFmt numFmtId="165" formatCode="0.00;\-0.00;\-"/>
@@ -573,13 +578,122 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -593,121 +707,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -977,7 +982,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -987,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="AA15" sqref="AA15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1014,203 +1019,203 @@
   <sheetData>
     <row r="1" spans="2:18" ht="409.6" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:18" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
     </row>
     <row r="3" spans="2:18" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
-      <c r="O3" s="38"/>
-      <c r="P3" s="38"/>
-      <c r="Q3" s="38"/>
-      <c r="R3" s="38"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
     </row>
     <row r="4" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="39"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
     </row>
     <row r="5" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="40" t="s">
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="41"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="N5" s="44"/>
-      <c r="O5" s="44"/>
-      <c r="P5" s="44"/>
-      <c r="Q5" s="44"/>
-      <c r="R5" s="44"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="18"/>
     </row>
     <row r="6" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="51"/>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="31" t="s">
+      <c r="B6" s="22"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="K6" s="32"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="43" t="s">
+      <c r="K6" s="15"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="N6" s="43"/>
-      <c r="O6" s="43"/>
-      <c r="P6" s="43"/>
-      <c r="Q6" s="43"/>
-      <c r="R6" s="43"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
     </row>
     <row r="7" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="36"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="27"/>
       <c r="J7" s="6"/>
       <c r="K7" s="29"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="43"/>
-      <c r="N7" s="43"/>
-      <c r="O7" s="43"/>
-      <c r="P7" s="43"/>
-      <c r="Q7" s="43"/>
-      <c r="R7" s="43"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
     </row>
     <row r="8" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30" t="s">
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="31" t="s">
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="K8" s="32"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="43" t="s">
+      <c r="K8" s="15"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="N8" s="43"/>
-      <c r="O8" s="43"/>
-      <c r="P8" s="43"/>
-      <c r="Q8" s="43"/>
-      <c r="R8" s="43"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="17"/>
     </row>
     <row r="9" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="47"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="34"/>
       <c r="J9" s="7"/>
       <c r="K9" s="29"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="43"/>
-      <c r="N9" s="43"/>
-      <c r="O9" s="43"/>
-      <c r="P9" s="43"/>
-      <c r="Q9" s="43"/>
-      <c r="R9" s="43"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="17"/>
     </row>
     <row r="10" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="36"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="27"/>
       <c r="J10" s="6"/>
       <c r="K10" s="29"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="43"/>
-      <c r="N10" s="43"/>
-      <c r="O10" s="43"/>
-      <c r="P10" s="43"/>
-      <c r="Q10" s="43"/>
-      <c r="R10" s="43"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="17"/>
     </row>
     <row r="11" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="2:18" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
@@ -1236,319 +1241,319 @@
     </row>
     <row r="13" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="24" t="s">
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="24"/>
-      <c r="L14" s="24"/>
-      <c r="M14" s="24"/>
-      <c r="N14" s="24"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="24"/>
-      <c r="R14" s="24"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="37"/>
+      <c r="M14" s="37"/>
+      <c r="N14" s="37"/>
+      <c r="O14" s="37"/>
+      <c r="P14" s="37"/>
+      <c r="Q14" s="37"/>
+      <c r="R14" s="37"/>
     </row>
     <row r="15" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="24"/>
-      <c r="M15" s="24"/>
-      <c r="N15" s="24"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="24"/>
-      <c r="R15" s="24"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="37"/>
+      <c r="N15" s="37"/>
+      <c r="O15" s="37"/>
+      <c r="P15" s="37"/>
+      <c r="Q15" s="37"/>
+      <c r="R15" s="37"/>
     </row>
     <row r="16" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
     </row>
     <row r="17" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="25"/>
-      <c r="O17" s="25"/>
-      <c r="P17" s="25"/>
-      <c r="Q17" s="25"/>
-      <c r="R17" s="25"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="38"/>
+      <c r="N17" s="38"/>
+      <c r="O17" s="38"/>
+      <c r="P17" s="38"/>
+      <c r="Q17" s="38"/>
+      <c r="R17" s="38"/>
     </row>
     <row r="18" spans="2:18" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="27" t="s">
+      <c r="C18" s="39"/>
+      <c r="D18" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
       <c r="H18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I18" s="27" t="s">
+      <c r="I18" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="J18" s="27"/>
-      <c r="K18" s="27" t="s">
+      <c r="J18" s="40"/>
+      <c r="K18" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="L18" s="27"/>
-      <c r="M18" s="27"/>
-      <c r="N18" s="27" t="s">
+      <c r="L18" s="40"/>
+      <c r="M18" s="40"/>
+      <c r="N18" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="O18" s="27"/>
-      <c r="P18" s="27"/>
-      <c r="Q18" s="23" t="s">
+      <c r="O18" s="40"/>
+      <c r="P18" s="40"/>
+      <c r="Q18" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="R18" s="23"/>
+      <c r="R18" s="35"/>
     </row>
     <row r="19" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="18" t="s">
+      <c r="C19" s="42"/>
+      <c r="D19" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
       <c r="H19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I19" s="18" t="s">
+      <c r="I19" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18" t="s">
+      <c r="J19" s="43"/>
+      <c r="K19" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18" t="s">
+      <c r="L19" s="43"/>
+      <c r="M19" s="43"/>
+      <c r="N19" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="19" t="s">
+      <c r="O19" s="43"/>
+      <c r="P19" s="43"/>
+      <c r="Q19" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="R19" s="19"/>
+      <c r="R19" s="44"/>
     </row>
     <row r="20" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="45"/>
+      <c r="D20" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="21" t="s">
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I20" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="3" t="s">
+      <c r="J20" s="45"/>
+      <c r="K20" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="L20" s="47"/>
+      <c r="M20" s="47"/>
+      <c r="N20" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="O20" s="41"/>
+      <c r="P20" s="41"/>
+      <c r="Q20" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="R20" s="41"/>
+    </row>
+    <row r="21" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H21" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="36"/>
+      <c r="O21" s="36"/>
+      <c r="Q21" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="R21" s="49"/>
+    </row>
+    <row r="22" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H22" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="I22" s="36"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="36"/>
+      <c r="M22" s="36"/>
+      <c r="N22" s="36"/>
+      <c r="O22" s="36"/>
+      <c r="Q22" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="I20" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="J20" s="20"/>
-      <c r="K20" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="L20" s="22"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="O20" s="16"/>
-      <c r="P20" s="16"/>
-      <c r="Q20" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="R20" s="16"/>
-    </row>
-    <row r="21" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H21" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="Q21" s="12" t="s">
+      <c r="R22" s="49"/>
+    </row>
+    <row r="23" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H23" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="I23" s="50"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="50"/>
+      <c r="L23" s="50"/>
+      <c r="M23" s="50"/>
+      <c r="N23" s="50"/>
+      <c r="O23" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="P23" s="51"/>
+      <c r="Q23" s="51"/>
+      <c r="R23" s="51"/>
+    </row>
+    <row r="24" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="R21" s="12"/>
-    </row>
-    <row r="22" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H22" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
-      <c r="Q22" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="R22" s="12"/>
-    </row>
-    <row r="23" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H23" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="P23" s="14"/>
-      <c r="Q23" s="14"/>
-      <c r="R23" s="14"/>
-    </row>
-    <row r="24" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="15" t="s">
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="52"/>
+      <c r="M24" s="52"/>
+      <c r="N24" s="52"/>
+      <c r="O24" s="52"/>
+      <c r="P24" s="52"/>
+      <c r="Q24" s="52"/>
+      <c r="R24" s="52"/>
+    </row>
+    <row r="25" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="15"/>
-    </row>
-    <row r="25" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="9"/>
-      <c r="P25" s="9"/>
-      <c r="Q25" s="9"/>
-      <c r="R25" s="9"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="53"/>
+      <c r="I25" s="53"/>
+      <c r="J25" s="53"/>
+      <c r="K25" s="53"/>
+      <c r="L25" s="53"/>
+      <c r="M25" s="53"/>
+      <c r="N25" s="53"/>
+      <c r="O25" s="53"/>
+      <c r="P25" s="53"/>
+      <c r="Q25" s="53"/>
+      <c r="R25" s="53"/>
     </row>
     <row r="26" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="9" t="s">
+      <c r="N27" s="53"/>
+      <c r="O27" s="53"/>
+      <c r="P27" s="53"/>
+      <c r="Q27" s="53"/>
+      <c r="R27" s="53"/>
+    </row>
+    <row r="28" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G28" s="48"/>
+      <c r="H28" s="48"/>
+      <c r="I28" s="48"/>
+      <c r="J28" s="48"/>
+      <c r="K28" s="48"/>
+      <c r="L28" s="48"/>
+    </row>
+    <row r="29" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="36"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="30"/>
+      <c r="L29" s="30"/>
+      <c r="M29" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="N27" s="9"/>
-      <c r="O27" s="9"/>
-      <c r="P27" s="9"/>
-      <c r="Q27" s="9"/>
-      <c r="R27" s="9"/>
-    </row>
-    <row r="28" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
-      <c r="L28" s="11"/>
-    </row>
-    <row r="29" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="9"/>
-      <c r="R29" s="9"/>
+      <c r="N29" s="53"/>
+      <c r="O29" s="53"/>
+      <c r="P29" s="53"/>
+      <c r="Q29" s="53"/>
+      <c r="R29" s="53"/>
     </row>
     <row r="30" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="48"/>
       <c r="I30" s="4"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
-      <c r="L30" s="11"/>
+      <c r="J30" s="48"/>
+      <c r="K30" s="48"/>
+      <c r="L30" s="48"/>
     </row>
     <row r="31" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I31" s="5" t="s">
@@ -1557,24 +1562,35 @@
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="B2:R2"/>
-    <mergeCell ref="B3:R3"/>
-    <mergeCell ref="C4:Q4"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="M6:R7"/>
-    <mergeCell ref="M5:R5"/>
-    <mergeCell ref="B5:I6"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B12:R12"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="K9:L10"/>
-    <mergeCell ref="B10:I10"/>
-    <mergeCell ref="B9:I9"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="M8:R10"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="M29:R29"/>
+    <mergeCell ref="G29:L29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="J30:L30"/>
+    <mergeCell ref="G28:L28"/>
+    <mergeCell ref="H21:O21"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="H22:O22"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="H23:N23"/>
+    <mergeCell ref="O23:R23"/>
+    <mergeCell ref="B24:R24"/>
+    <mergeCell ref="B25:R25"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="M27:R27"/>
+    <mergeCell ref="G27:L27"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="N20:P20"/>
     <mergeCell ref="Q18:R18"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="E14:R14"/>
@@ -1587,35 +1603,24 @@
     <mergeCell ref="I18:J18"/>
     <mergeCell ref="K18:M18"/>
     <mergeCell ref="N18:P18"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="N19:P19"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:G20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="G28:L28"/>
-    <mergeCell ref="H21:O21"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="H22:O22"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="H23:N23"/>
-    <mergeCell ref="O23:R23"/>
-    <mergeCell ref="B24:R24"/>
-    <mergeCell ref="B25:R25"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="M27:R27"/>
-    <mergeCell ref="G27:L27"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="M29:R29"/>
-    <mergeCell ref="G29:L29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="J30:L30"/>
+    <mergeCell ref="B12:R12"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="K9:L10"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B9:I9"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="M8:R10"/>
+    <mergeCell ref="B2:R2"/>
+    <mergeCell ref="B3:R3"/>
+    <mergeCell ref="C4:Q4"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="M6:R7"/>
+    <mergeCell ref="M5:R5"/>
+    <mergeCell ref="B5:I6"/>
+    <mergeCell ref="B7:I7"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="90" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
adding support for float_point_product_quantity
</commit_message>
<xml_diff>
--- a/application/views/rpt/ru/doc/schet.xlsx
+++ b/application/views/rpt/ru/doc/schet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1476" yWindow="36" windowWidth="7452" windowHeight="6240"/>
+    <workbookView xWindow="2592" yWindow="36" windowWidth="7452" windowHeight="6240"/>
   </bookViews>
   <sheets>
     <sheet name="Счет" sheetId="1" r:id="rId1"/>
@@ -190,8 +190,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0;\-0;\-"/>
+  <numFmts count="1">
     <numFmt numFmtId="165" formatCode="0.00;\-0.00;\-"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
@@ -602,59 +601,117 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -669,114 +726,56 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1061,7 +1060,7 @@
   <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="Y21" sqref="Y21"/>
+      <selection activeCell="S31" sqref="S31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1087,541 +1086,541 @@
   <sheetData>
     <row r="1" spans="2:18" ht="409.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:18" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="61"/>
+      <c r="O2" s="61"/>
+      <c r="P2" s="61"/>
+      <c r="Q2" s="61"/>
+      <c r="R2" s="61"/>
     </row>
     <row r="3" spans="2:18" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="62"/>
+      <c r="K3" s="62"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="62"/>
+      <c r="N3" s="62"/>
+      <c r="O3" s="62"/>
+      <c r="P3" s="62"/>
+      <c r="Q3" s="62"/>
+      <c r="R3" s="62"/>
     </row>
     <row r="4" spans="2:18" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="57" t="s">
+      <c r="C4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
-      <c r="M4" s="57"/>
-      <c r="N4" s="57"/>
-      <c r="O4" s="57"/>
-      <c r="P4" s="57"/>
-      <c r="Q4" s="57"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
     </row>
     <row r="5" spans="2:18" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="64" t="s">
+      <c r="B5" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="61" t="s">
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="62"/>
-      <c r="L5" s="63"/>
-      <c r="M5" s="58" t="s">
+      <c r="K5" s="27"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="N5" s="59"/>
-      <c r="O5" s="59"/>
-      <c r="P5" s="59"/>
-      <c r="Q5" s="59"/>
-      <c r="R5" s="60"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="24"/>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="25"/>
     </row>
     <row r="6" spans="2:18" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="67"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="69"/>
-      <c r="J6" s="51" t="s">
+      <c r="B6" s="32"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K6" s="52"/>
-      <c r="L6" s="53"/>
-      <c r="M6" s="42" t="s">
+      <c r="K6" s="21"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="N6" s="43"/>
-      <c r="O6" s="43"/>
-      <c r="P6" s="43"/>
-      <c r="Q6" s="43"/>
-      <c r="R6" s="44"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="16"/>
     </row>
     <row r="7" spans="2:18" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="35"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="13"/>
       <c r="J7" s="6"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="48"/>
-      <c r="N7" s="49"/>
-      <c r="O7" s="49"/>
-      <c r="P7" s="49"/>
-      <c r="Q7" s="49"/>
-      <c r="R7" s="50"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="19"/>
     </row>
     <row r="8" spans="2:18" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="55"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="54" t="s">
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="55"/>
-      <c r="H8" s="55"/>
-      <c r="I8" s="56"/>
-      <c r="J8" s="51" t="s">
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="K8" s="52"/>
-      <c r="L8" s="53"/>
-      <c r="M8" s="42" t="s">
+      <c r="K8" s="21"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="N8" s="43"/>
-      <c r="O8" s="43"/>
-      <c r="P8" s="43"/>
-      <c r="Q8" s="43"/>
-      <c r="R8" s="44"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="16"/>
     </row>
     <row r="9" spans="2:18" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="41"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="39"/>
       <c r="J9" s="7"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="37"/>
-      <c r="M9" s="45"/>
-      <c r="N9" s="46"/>
-      <c r="O9" s="46"/>
-      <c r="P9" s="46"/>
-      <c r="Q9" s="46"/>
-      <c r="R9" s="47"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="41"/>
+      <c r="O9" s="41"/>
+      <c r="P9" s="41"/>
+      <c r="Q9" s="41"/>
+      <c r="R9" s="42"/>
     </row>
     <row r="10" spans="2:18" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="35"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="13"/>
       <c r="J10" s="6"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="48"/>
-      <c r="N10" s="49"/>
-      <c r="O10" s="49"/>
-      <c r="P10" s="49"/>
-      <c r="Q10" s="49"/>
-      <c r="R10" s="50"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="19"/>
     </row>
     <row r="11" spans="2:18" ht="79.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="2:18" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="60"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="60"/>
+      <c r="M12" s="60"/>
+      <c r="N12" s="60"/>
+      <c r="O12" s="60"/>
+      <c r="P12" s="60"/>
+      <c r="Q12" s="60"/>
+      <c r="R12" s="60"/>
     </row>
     <row r="13" spans="2:18" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="14" t="s">
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="65"/>
+      <c r="J14" s="65"/>
+      <c r="K14" s="65"/>
+      <c r="L14" s="65"/>
+      <c r="M14" s="65"/>
+      <c r="N14" s="65"/>
+      <c r="O14" s="65"/>
+      <c r="P14" s="65"/>
+      <c r="Q14" s="65"/>
+      <c r="R14" s="65"/>
     </row>
     <row r="15" spans="2:18" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="14" t="s">
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="65"/>
+      <c r="J15" s="65"/>
+      <c r="K15" s="65"/>
+      <c r="L15" s="65"/>
+      <c r="M15" s="65"/>
+      <c r="N15" s="65"/>
+      <c r="O15" s="65"/>
+      <c r="P15" s="65"/>
+      <c r="Q15" s="65"/>
+      <c r="R15" s="65"/>
     </row>
     <row r="16" spans="2:18" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
     </row>
     <row r="17" spans="1:18" ht="14.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="15"/>
+      <c r="L17" s="66"/>
+      <c r="M17" s="66"/>
+      <c r="N17" s="66"/>
+      <c r="O17" s="66"/>
+      <c r="P17" s="66"/>
+      <c r="Q17" s="66"/>
+      <c r="R17" s="66"/>
     </row>
     <row r="18" spans="1:18" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="17" t="s">
+      <c r="C18" s="67"/>
+      <c r="D18" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
+      <c r="E18" s="68"/>
+      <c r="F18" s="68"/>
+      <c r="G18" s="68"/>
       <c r="H18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I18" s="17" t="s">
+      <c r="I18" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17" t="s">
+      <c r="J18" s="68"/>
+      <c r="K18" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="17" t="s">
+      <c r="L18" s="68"/>
+      <c r="M18" s="68"/>
+      <c r="N18" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="O18" s="17"/>
-      <c r="P18" s="17"/>
-      <c r="Q18" s="12" t="s">
+      <c r="O18" s="68"/>
+      <c r="P18" s="68"/>
+      <c r="Q18" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="R18" s="12"/>
+      <c r="R18" s="64"/>
     </row>
     <row r="19" spans="1:18" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="21" t="s">
+      <c r="C19" s="55"/>
+      <c r="D19" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="56"/>
       <c r="H19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I19" s="21" t="s">
+      <c r="I19" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="J19" s="21"/>
-      <c r="K19" s="21" t="s">
+      <c r="J19" s="56"/>
+      <c r="K19" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="L19" s="21"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="21" t="s">
+      <c r="L19" s="56"/>
+      <c r="M19" s="56"/>
+      <c r="N19" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="O19" s="21"/>
-      <c r="P19" s="21"/>
-      <c r="Q19" s="22" t="s">
+      <c r="O19" s="56"/>
+      <c r="P19" s="56"/>
+      <c r="Q19" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="R19" s="22"/>
+      <c r="R19" s="57"/>
     </row>
     <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="24" t="s">
+      <c r="C20" s="58"/>
+      <c r="D20" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="59"/>
       <c r="H20" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I20" s="23" t="s">
+      <c r="I20" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="J20" s="23"/>
-      <c r="K20" s="25" t="s">
+      <c r="J20" s="58"/>
+      <c r="K20" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="L20" s="25"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="18" t="s">
+      <c r="L20" s="69"/>
+      <c r="M20" s="69"/>
+      <c r="N20" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="O20" s="19"/>
-      <c r="P20" s="19"/>
-      <c r="Q20" s="18" t="s">
+      <c r="O20" s="54"/>
+      <c r="P20" s="54"/>
+      <c r="Q20" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="R20" s="19"/>
+      <c r="R20" s="54"/>
     </row>
     <row r="21" spans="1:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H21" s="13" t="s">
+      <c r="H21" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="Q21" s="27" t="s">
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="46"/>
+      <c r="N21" s="46"/>
+      <c r="O21" s="46"/>
+      <c r="Q21" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="R21" s="27"/>
+      <c r="R21" s="49"/>
     </row>
     <row r="22" spans="1:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H22" s="13" t="s">
+      <c r="H22" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="Q22" s="27" t="s">
+      <c r="I22" s="46"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="46"/>
+      <c r="L22" s="46"/>
+      <c r="M22" s="46"/>
+      <c r="N22" s="46"/>
+      <c r="O22" s="46"/>
+      <c r="Q22" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="R22" s="27"/>
+      <c r="R22" s="49"/>
     </row>
     <row r="23" spans="1:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H23" s="28" t="s">
+      <c r="H23" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="28"/>
-      <c r="M23" s="28"/>
-      <c r="N23" s="28"/>
-      <c r="O23" s="29" t="s">
+      <c r="I23" s="50"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="50"/>
+      <c r="L23" s="50"/>
+      <c r="M23" s="50"/>
+      <c r="N23" s="50"/>
+      <c r="O23" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="P23" s="29"/>
-      <c r="Q23" s="29"/>
-      <c r="R23" s="29"/>
+      <c r="P23" s="51"/>
+      <c r="Q23" s="51"/>
+      <c r="R23" s="51"/>
     </row>
     <row r="24" spans="1:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="30"/>
-      <c r="J24" s="30"/>
-      <c r="K24" s="30"/>
-      <c r="L24" s="30"/>
-      <c r="M24" s="30"/>
-      <c r="N24" s="30"/>
-      <c r="O24" s="30"/>
-      <c r="P24" s="30"/>
-      <c r="Q24" s="30"/>
-      <c r="R24" s="30"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="52"/>
+      <c r="M24" s="52"/>
+      <c r="N24" s="52"/>
+      <c r="O24" s="52"/>
+      <c r="P24" s="52"/>
+      <c r="Q24" s="52"/>
+      <c r="R24" s="52"/>
     </row>
     <row r="25" spans="1:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="31"/>
-      <c r="L25" s="31"/>
-      <c r="M25" s="31"/>
-      <c r="N25" s="31"/>
-      <c r="O25" s="31"/>
-      <c r="P25" s="31"/>
-      <c r="Q25" s="31"/>
-      <c r="R25" s="31"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="47"/>
+      <c r="I25" s="47"/>
+      <c r="J25" s="47"/>
+      <c r="K25" s="47"/>
+      <c r="L25" s="47"/>
+      <c r="M25" s="47"/>
+      <c r="N25" s="47"/>
+      <c r="O25" s="47"/>
+      <c r="P25" s="47"/>
+      <c r="Q25" s="47"/>
+      <c r="R25" s="47"/>
     </row>
     <row r="26" spans="1:18" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="32"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="32"/>
-      <c r="J27" s="32"/>
-      <c r="K27" s="32"/>
-      <c r="L27" s="32"/>
-      <c r="M27" s="31" t="s">
+      <c r="C27" s="46"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="N27" s="31"/>
-      <c r="O27" s="31"/>
-      <c r="P27" s="31"/>
-      <c r="Q27" s="31"/>
-      <c r="R27" s="31"/>
+      <c r="N27" s="47"/>
+      <c r="O27" s="47"/>
+      <c r="P27" s="47"/>
+      <c r="Q27" s="47"/>
+      <c r="R27" s="47"/>
     </row>
     <row r="28" spans="1:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="26"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="48"/>
+      <c r="I28" s="48"/>
+      <c r="J28" s="48"/>
+      <c r="K28" s="48"/>
+      <c r="L28" s="48"/>
     </row>
     <row r="29" spans="1:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="32"/>
-      <c r="K29" s="32"/>
-      <c r="L29" s="32"/>
-      <c r="M29" s="31" t="s">
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="N29" s="31"/>
-      <c r="O29" s="31"/>
-      <c r="P29" s="31"/>
-      <c r="Q29" s="31"/>
-      <c r="R29" s="31"/>
+      <c r="N29" s="47"/>
+      <c r="O29" s="47"/>
+      <c r="P29" s="47"/>
+      <c r="Q29" s="47"/>
+      <c r="R29" s="47"/>
     </row>
     <row r="30" spans="1:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="48"/>
       <c r="I30" s="4"/>
-      <c r="J30" s="26"/>
-      <c r="K30" s="26"/>
-      <c r="L30" s="26"/>
+      <c r="J30" s="48"/>
+      <c r="K30" s="48"/>
+      <c r="L30" s="48"/>
     </row>
     <row r="31" spans="1:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I31" s="5" t="s">
@@ -1629,73 +1628,29 @@
       </c>
     </row>
     <row r="32" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="11"/>
-      <c r="L32" s="11"/>
-      <c r="M32" s="11"/>
-      <c r="N32" s="11"/>
-      <c r="O32" s="11"/>
-      <c r="P32" s="11"/>
-      <c r="Q32" s="11"/>
-      <c r="R32" s="11"/>
+      <c r="B32" s="63"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="63"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="63"/>
+      <c r="I32" s="63"/>
+      <c r="J32" s="63"/>
+      <c r="K32" s="63"/>
+      <c r="L32" s="63"/>
+      <c r="M32" s="63"/>
+      <c r="N32" s="63"/>
+      <c r="O32" s="63"/>
+      <c r="P32" s="63"/>
+      <c r="Q32" s="63"/>
+      <c r="R32" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="C4:Q4"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="M6:R7"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="M5:R5"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="B5:I6"/>
-    <mergeCell ref="B10:I10"/>
-    <mergeCell ref="K9:L10"/>
-    <mergeCell ref="B9:I9"/>
-    <mergeCell ref="M8:R10"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="M29:R29"/>
-    <mergeCell ref="G29:L29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="J30:L30"/>
-    <mergeCell ref="G28:L28"/>
-    <mergeCell ref="H21:O21"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="H22:O22"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="H23:N23"/>
-    <mergeCell ref="O23:R23"/>
-    <mergeCell ref="B24:R24"/>
-    <mergeCell ref="B25:R25"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="M27:R27"/>
-    <mergeCell ref="G27:L27"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="N19:P19"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:G20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="N20:P20"/>
     <mergeCell ref="B12:R12"/>
     <mergeCell ref="B2:R2"/>
     <mergeCell ref="B3:R3"/>
@@ -1712,6 +1667,50 @@
     <mergeCell ref="I18:J18"/>
     <mergeCell ref="K18:M18"/>
     <mergeCell ref="N18:P18"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="G28:L28"/>
+    <mergeCell ref="H21:O21"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="H22:O22"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="H23:N23"/>
+    <mergeCell ref="O23:R23"/>
+    <mergeCell ref="B24:R24"/>
+    <mergeCell ref="B25:R25"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="M27:R27"/>
+    <mergeCell ref="G27:L27"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="M29:R29"/>
+    <mergeCell ref="G29:L29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="J30:L30"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="K9:L10"/>
+    <mergeCell ref="B9:I9"/>
+    <mergeCell ref="M8:R10"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="C4:Q4"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="M6:R7"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="M5:R5"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="B5:I6"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="90" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
bugfixes and working on moedelo sync
</commit_message>
<xml_diff>
--- a/application/views/rpt/ru/doc/schet.xlsx
+++ b/application/views/rpt/ru/doc/schet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3708" yWindow="36" windowWidth="7452" windowHeight="6240"/>
+    <workbookView xWindow="4824" yWindow="36" windowWidth="7452" windowHeight="6240"/>
   </bookViews>
   <sheets>
     <sheet name="Счет" sheetId="1" r:id="rId1"/>
@@ -584,7 +584,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -592,73 +592,131 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -668,116 +726,70 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1063,7 +1075,7 @@
   <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22:O22"/>
+      <selection activeCell="B24" sqref="B24:R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1089,615 +1101,571 @@
   <sheetData>
     <row r="1" spans="2:18" ht="409.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:18" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="62"/>
     </row>
     <row r="3" spans="2:18" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="63"/>
+      <c r="N3" s="63"/>
+      <c r="O3" s="63"/>
+      <c r="P3" s="63"/>
+      <c r="Q3" s="63"/>
+      <c r="R3" s="63"/>
     </row>
     <row r="4" spans="2:18" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="57" t="s">
+      <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
-      <c r="M4" s="57"/>
-      <c r="N4" s="57"/>
-      <c r="O4" s="57"/>
-      <c r="P4" s="57"/>
-      <c r="Q4" s="57"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
     </row>
     <row r="5" spans="2:18" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="64" t="s">
+      <c r="B5" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="61" t="s">
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="62"/>
-      <c r="L5" s="63"/>
-      <c r="M5" s="58" t="s">
+      <c r="K5" s="26"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="N5" s="59"/>
-      <c r="O5" s="59"/>
-      <c r="P5" s="59"/>
-      <c r="Q5" s="59"/>
-      <c r="R5" s="60"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="24"/>
     </row>
     <row r="6" spans="2:18" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="67"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="69"/>
-      <c r="J6" s="51" t="s">
+      <c r="B6" s="31"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="K6" s="52"/>
-      <c r="L6" s="53"/>
-      <c r="M6" s="42" t="s">
+      <c r="K6" s="20"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="N6" s="43"/>
-      <c r="O6" s="43"/>
-      <c r="P6" s="43"/>
-      <c r="Q6" s="43"/>
-      <c r="R6" s="44"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="15"/>
     </row>
     <row r="7" spans="2:18" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="48"/>
-      <c r="N7" s="49"/>
-      <c r="O7" s="49"/>
-      <c r="P7" s="49"/>
-      <c r="Q7" s="49"/>
-      <c r="R7" s="50"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="18"/>
     </row>
     <row r="8" spans="2:18" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="55"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="54" t="s">
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="55"/>
-      <c r="H8" s="55"/>
-      <c r="I8" s="56"/>
-      <c r="J8" s="51" t="s">
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="K8" s="52"/>
-      <c r="L8" s="53"/>
-      <c r="M8" s="42" t="s">
+      <c r="K8" s="20"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="N8" s="43"/>
-      <c r="O8" s="43"/>
-      <c r="P8" s="43"/>
-      <c r="Q8" s="43"/>
-      <c r="R8" s="44"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="15"/>
     </row>
     <row r="9" spans="2:18" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="37"/>
-      <c r="M9" s="45"/>
-      <c r="N9" s="46"/>
-      <c r="O9" s="46"/>
-      <c r="P9" s="46"/>
-      <c r="Q9" s="46"/>
-      <c r="R9" s="47"/>
-    </row>
-    <row r="10" spans="2:18" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="33" t="s">
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="39"/>
+      <c r="N9" s="40"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="41"/>
+    </row>
+    <row r="10" spans="2:18" ht="39.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="48"/>
-      <c r="N10" s="49"/>
-      <c r="O10" s="49"/>
-      <c r="P10" s="49"/>
-      <c r="Q10" s="49"/>
-      <c r="R10" s="50"/>
-    </row>
-    <row r="11" spans="2:18" ht="79.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="18"/>
+    </row>
+    <row r="11" spans="2:18" ht="40.799999999999997" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="2:18" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="61"/>
+      <c r="J12" s="61"/>
+      <c r="K12" s="61"/>
+      <c r="L12" s="61"/>
+      <c r="M12" s="61"/>
+      <c r="N12" s="61"/>
+      <c r="O12" s="61"/>
+      <c r="P12" s="61"/>
+      <c r="Q12" s="61"/>
+      <c r="R12" s="61"/>
     </row>
     <row r="13" spans="2:18" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="2:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="14" t="s">
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="66"/>
+      <c r="H14" s="66"/>
+      <c r="I14" s="66"/>
+      <c r="J14" s="66"/>
+      <c r="K14" s="66"/>
+      <c r="L14" s="66"/>
+      <c r="M14" s="66"/>
+      <c r="N14" s="66"/>
+      <c r="O14" s="66"/>
+      <c r="P14" s="66"/>
+      <c r="Q14" s="66"/>
+      <c r="R14" s="66"/>
     </row>
     <row r="15" spans="2:18" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="14" t="s">
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="66"/>
+      <c r="H15" s="66"/>
+      <c r="I15" s="66"/>
+      <c r="J15" s="66"/>
+      <c r="K15" s="66"/>
+      <c r="L15" s="66"/>
+      <c r="M15" s="66"/>
+      <c r="N15" s="66"/>
+      <c r="O15" s="66"/>
+      <c r="P15" s="66"/>
+      <c r="Q15" s="66"/>
+      <c r="R15" s="66"/>
     </row>
     <row r="16" spans="2:18" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
     </row>
     <row r="17" spans="1:18" ht="14.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="15"/>
+      <c r="L17" s="67"/>
+      <c r="M17" s="67"/>
+      <c r="N17" s="67"/>
+      <c r="O17" s="67"/>
+      <c r="P17" s="67"/>
+      <c r="Q17" s="67"/>
+      <c r="R17" s="67"/>
     </row>
     <row r="18" spans="1:18" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="17" t="s">
+      <c r="C18" s="68"/>
+      <c r="D18" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="69"/>
       <c r="H18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I18" s="17" t="s">
+      <c r="I18" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17" t="s">
+      <c r="J18" s="69"/>
+      <c r="K18" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="17" t="s">
+      <c r="L18" s="69"/>
+      <c r="M18" s="69"/>
+      <c r="N18" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="O18" s="17"/>
-      <c r="P18" s="17"/>
-      <c r="Q18" s="12" t="s">
+      <c r="O18" s="69"/>
+      <c r="P18" s="69"/>
+      <c r="Q18" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="R18" s="12"/>
+      <c r="R18" s="65"/>
     </row>
     <row r="19" spans="1:18" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="21" t="s">
+      <c r="C19" s="55"/>
+      <c r="D19" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="56"/>
       <c r="H19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I19" s="21" t="s">
+      <c r="I19" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="J19" s="21"/>
-      <c r="K19" s="21" t="s">
+      <c r="J19" s="56"/>
+      <c r="K19" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="L19" s="21"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="21" t="s">
+      <c r="L19" s="56"/>
+      <c r="M19" s="56"/>
+      <c r="N19" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="O19" s="21"/>
-      <c r="P19" s="21"/>
-      <c r="Q19" s="22" t="s">
+      <c r="O19" s="56"/>
+      <c r="P19" s="56"/>
+      <c r="Q19" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="R19" s="22"/>
+      <c r="R19" s="57"/>
     </row>
     <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="24" t="s">
+      <c r="C20" s="58"/>
+      <c r="D20" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="3" t="s">
+      <c r="E20" s="59"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="59"/>
+      <c r="H20" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="I20" s="23" t="s">
+      <c r="I20" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="J20" s="23"/>
-      <c r="K20" s="25" t="s">
+      <c r="J20" s="58"/>
+      <c r="K20" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="L20" s="25"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="18" t="s">
+      <c r="L20" s="60"/>
+      <c r="M20" s="60"/>
+      <c r="N20" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="O20" s="19"/>
-      <c r="P20" s="19"/>
-      <c r="Q20" s="18" t="s">
+      <c r="O20" s="54"/>
+      <c r="P20" s="54"/>
+      <c r="Q20" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="R20" s="19"/>
+      <c r="R20" s="54"/>
     </row>
     <row r="21" spans="1:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H21" s="13" t="s">
+      <c r="H21" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="Q21" s="27" t="s">
+      <c r="I21" s="45"/>
+      <c r="J21" s="45"/>
+      <c r="K21" s="45"/>
+      <c r="L21" s="45"/>
+      <c r="M21" s="45"/>
+      <c r="N21" s="45"/>
+      <c r="O21" s="45"/>
+      <c r="Q21" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="R21" s="27"/>
+      <c r="R21" s="48"/>
     </row>
     <row r="22" spans="1:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H22" s="70" t="s">
+      <c r="H22" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="Q22" s="27" t="s">
+      <c r="I22" s="45"/>
+      <c r="J22" s="45"/>
+      <c r="K22" s="45"/>
+      <c r="L22" s="45"/>
+      <c r="M22" s="45"/>
+      <c r="N22" s="45"/>
+      <c r="O22" s="45"/>
+      <c r="Q22" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="R22" s="27"/>
+      <c r="R22" s="48"/>
     </row>
     <row r="23" spans="1:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H23" s="28" t="s">
+      <c r="H23" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="28"/>
-      <c r="M23" s="28"/>
-      <c r="N23" s="28"/>
-      <c r="O23" s="29" t="s">
+      <c r="I23" s="50"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="50"/>
+      <c r="L23" s="50"/>
+      <c r="M23" s="50"/>
+      <c r="N23" s="50"/>
+      <c r="O23" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="P23" s="29"/>
-      <c r="Q23" s="29"/>
-      <c r="R23" s="29"/>
+      <c r="P23" s="51"/>
+      <c r="Q23" s="51"/>
+      <c r="R23" s="51"/>
     </row>
     <row r="24" spans="1:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="30"/>
-      <c r="J24" s="30"/>
-      <c r="K24" s="30"/>
-      <c r="L24" s="30"/>
-      <c r="M24" s="30"/>
-      <c r="N24" s="30"/>
-      <c r="O24" s="30"/>
-      <c r="P24" s="30"/>
-      <c r="Q24" s="30"/>
-      <c r="R24" s="30"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="52"/>
+      <c r="M24" s="52"/>
+      <c r="N24" s="52"/>
+      <c r="O24" s="52"/>
+      <c r="P24" s="52"/>
+      <c r="Q24" s="52"/>
+      <c r="R24" s="52"/>
     </row>
     <row r="25" spans="1:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="31"/>
-      <c r="L25" s="31"/>
-      <c r="M25" s="31"/>
-      <c r="N25" s="31"/>
-      <c r="O25" s="31"/>
-      <c r="P25" s="31"/>
-      <c r="Q25" s="31"/>
-      <c r="R25" s="31"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="46"/>
+      <c r="L25" s="46"/>
+      <c r="M25" s="46"/>
+      <c r="N25" s="46"/>
+      <c r="O25" s="46"/>
+      <c r="P25" s="46"/>
+      <c r="Q25" s="46"/>
+      <c r="R25" s="46"/>
     </row>
     <row r="26" spans="1:18" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="32"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="32"/>
-      <c r="J27" s="32"/>
-      <c r="K27" s="32"/>
-      <c r="L27" s="32"/>
-      <c r="M27" s="31" t="s">
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="N27" s="31"/>
-      <c r="O27" s="31"/>
-      <c r="P27" s="31"/>
-      <c r="Q27" s="31"/>
-      <c r="R27" s="31"/>
+      <c r="N27" s="46"/>
+      <c r="O27" s="46"/>
+      <c r="P27" s="46"/>
+      <c r="Q27" s="46"/>
+      <c r="R27" s="46"/>
     </row>
     <row r="28" spans="1:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="26"/>
+      <c r="G28" s="47"/>
+      <c r="H28" s="47"/>
+      <c r="I28" s="47"/>
+      <c r="J28" s="47"/>
+      <c r="K28" s="47"/>
+      <c r="L28" s="47"/>
     </row>
     <row r="29" spans="1:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="32"/>
-      <c r="K29" s="32"/>
-      <c r="L29" s="32"/>
-      <c r="M29" s="31" t="s">
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="N29" s="31"/>
-      <c r="O29" s="31"/>
-      <c r="P29" s="31"/>
-      <c r="Q29" s="31"/>
-      <c r="R29" s="31"/>
+      <c r="N29" s="46"/>
+      <c r="O29" s="46"/>
+      <c r="P29" s="46"/>
+      <c r="Q29" s="46"/>
+      <c r="R29" s="46"/>
     </row>
     <row r="30" spans="1:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="26"/>
-      <c r="K30" s="26"/>
-      <c r="L30" s="26"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="47"/>
+      <c r="K30" s="47"/>
+      <c r="L30" s="47"/>
     </row>
     <row r="31" spans="1:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I31" s="5" t="s">
+      <c r="I31" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="11"/>
-      <c r="L32" s="11"/>
-      <c r="M32" s="11"/>
-      <c r="N32" s="11"/>
-      <c r="O32" s="11"/>
-      <c r="P32" s="11"/>
-      <c r="Q32" s="11"/>
-      <c r="R32" s="11"/>
+      <c r="B32" s="64"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="64"/>
+      <c r="E32" s="64"/>
+      <c r="F32" s="64"/>
+      <c r="G32" s="64"/>
+      <c r="H32" s="64"/>
+      <c r="I32" s="64"/>
+      <c r="J32" s="64"/>
+      <c r="K32" s="64"/>
+      <c r="L32" s="64"/>
+      <c r="M32" s="64"/>
+      <c r="N32" s="64"/>
+      <c r="O32" s="64"/>
+      <c r="P32" s="64"/>
+      <c r="Q32" s="64"/>
+      <c r="R32" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="C4:Q4"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="M6:R7"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="M5:R5"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="B5:I6"/>
-    <mergeCell ref="B10:I10"/>
-    <mergeCell ref="K9:L10"/>
-    <mergeCell ref="B9:I9"/>
-    <mergeCell ref="M8:R10"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="M29:R29"/>
-    <mergeCell ref="G29:L29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="J30:L30"/>
-    <mergeCell ref="G28:L28"/>
-    <mergeCell ref="H21:O21"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="H22:O22"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="H23:N23"/>
-    <mergeCell ref="O23:R23"/>
-    <mergeCell ref="B24:R24"/>
-    <mergeCell ref="B25:R25"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="M27:R27"/>
-    <mergeCell ref="G27:L27"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="N19:P19"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:G20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="N20:P20"/>
     <mergeCell ref="B12:R12"/>
     <mergeCell ref="B2:R2"/>
     <mergeCell ref="B3:R3"/>
@@ -1714,6 +1682,50 @@
     <mergeCell ref="I18:J18"/>
     <mergeCell ref="K18:M18"/>
     <mergeCell ref="N18:P18"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="G28:L28"/>
+    <mergeCell ref="H21:O21"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="H22:O22"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="H23:N23"/>
+    <mergeCell ref="O23:R23"/>
+    <mergeCell ref="B24:R24"/>
+    <mergeCell ref="B25:R25"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="M27:R27"/>
+    <mergeCell ref="G27:L27"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="M29:R29"/>
+    <mergeCell ref="G29:L29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="J30:L30"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="K9:L10"/>
+    <mergeCell ref="B9:I9"/>
+    <mergeCell ref="M8:R10"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="C4:Q4"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="M6:R7"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="M5:R5"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="B5:I6"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="90" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>